<commit_message>
New validation in the check adjustment logic
</commit_message>
<xml_diff>
--- a/Documentation/Lists/Margins List.xlsx
+++ b/Documentation/Lists/Margins List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/Returns Taxpayer documentation/Lists/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.martinez\Documents\githubProject-IRBot\STS_InternalReviewBot\Documentation\Lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{5A8559F6-A36E-481C-AABE-A2BCD3D8FC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A27D884D-3E9D-4363-B607-A22E121139F1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE94888-5EF0-41B4-8E71-46EDB3EC8DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A226995F-052D-4F34-A143-258D99EE306B}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15840" xr2:uid="{A226995F-052D-4F34-A143-258D99EE306B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -130,10 +130,10 @@
     <t>WA REV-40 2406Q</t>
   </si>
   <si>
-    <t>Questions</t>
-  </si>
-  <si>
     <t>CO</t>
+  </si>
+  <si>
+    <t>CO DR-0100 XML</t>
   </si>
 </sst>
 </file>
@@ -141,7 +141,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -174,7 +174,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -190,10 +190,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -493,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B34C16A-BF47-4145-A119-63FE4C597FED}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,10 +558,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -709,11 +708,6 @@
       </c>
       <c r="C19" s="1">
         <v>10000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>